<commit_message>
End of day 25.06
</commit_message>
<xml_diff>
--- a/21.06 Компоновочная схема.xlsx
+++ b/21.06 Компоновочная схема.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RomodanEA\Desktop\Проектная практика\ProjectPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3701EA-53C6-4D11-8D1F-2977D5351DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E27E5C-A69B-4865-A4E9-212A13748AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="СборНагрузок" sheetId="1" r:id="rId1"/>
-    <sheet name="РасчётБалок" sheetId="2" r:id="rId2"/>
-    <sheet name="РасчетБалок" sheetId="3" r:id="rId3"/>
+    <sheet name="РасчетБалок" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>№ п/п</t>
   </si>
@@ -138,21 +137,6 @@
     <t>СП 20.13330.2016</t>
   </si>
   <si>
-    <t>Величина</t>
-  </si>
-  <si>
-    <t>Норматив</t>
-  </si>
-  <si>
-    <t>Расчётная</t>
-  </si>
-  <si>
-    <t>Единица</t>
-  </si>
-  <si>
-    <t>Второстепенные балки - ГОСТ 30245-2012</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -183,8 +167,20 @@
     </r>
   </si>
   <si>
+    <t>Wx</t>
+  </si>
+  <si>
+    <t>Jx</t>
+  </si>
+  <si>
+    <t>Mx</t>
+  </si>
+  <si>
+    <t>σ</t>
+  </si>
+  <si>
     <r>
-      <t>м</t>
+      <t>кг/см</t>
     </r>
     <r>
       <rPr>
@@ -194,7 +190,125 @@
         <rFont val="Inter"/>
         <charset val="204"/>
       </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>кг*см</t>
+  </si>
+  <si>
+    <r>
+      <t>см</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Inter"/>
+        <charset val="204"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <t>cм</t>
+  </si>
+  <si>
+    <t>Дано</t>
+  </si>
+  <si>
+    <t>см</t>
+  </si>
+  <si>
+    <r>
+      <t>см</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Inter"/>
+        <charset val="204"/>
+      </rPr>
       <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t>кг/см</t>
+  </si>
+  <si>
+    <t>Норма</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>γ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>с</t>
+    </r>
+  </si>
+  <si>
+    <t>Ry</t>
+  </si>
+  <si>
+    <t>160х160х7</t>
+  </si>
+  <si>
+    <t>Расчёт Jx</t>
+  </si>
+  <si>
+    <t>Расчёт Wx</t>
+  </si>
+  <si>
+    <t>20Б0</t>
+  </si>
+  <si>
+    <r>
+      <t>J</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>тр</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>тр</t>
     </r>
   </si>
   <si>
@@ -209,254 +323,15 @@
         <rFont val="Inter"/>
         <charset val="204"/>
       </rPr>
-      <t>4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Макс. прогиб &lt; 1/200*</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>l</t>
-    </r>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>✓</t>
-  </si>
-  <si>
-    <t>✗</t>
-  </si>
-  <si>
-    <t>Проверка на прочность при изгибе</t>
-  </si>
-  <si>
-    <t>Wx</t>
-  </si>
-  <si>
-    <t>Jx</t>
-  </si>
-  <si>
-    <t>σ</t>
-  </si>
-  <si>
-    <r>
-      <t>σ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>max</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>max</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>W</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>max</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>J</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>x</t>
-    </r>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>≤</t>
-  </si>
-  <si>
-    <r>
-      <t>кг/см</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Inter"/>
-        <charset val="204"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>кг/cм</t>
-  </si>
-  <si>
-    <t>кг*см</t>
-  </si>
-  <si>
-    <r>
-      <t>см</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Inter"/>
-        <charset val="204"/>
-      </rPr>
       <t>3</t>
     </r>
-  </si>
-  <si>
-    <t>СТД  НОМЕР              ИНФОРМАЦИЯ
-ГОСТ 27772-2015         σ
-ГОСТ 30245-2012         Jx, Wx, a, t
-СП   16.13330.2017      Уc, E</t>
-  </si>
-  <si>
-    <r>
-      <t>кг/cм</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Inter"/>
-        <charset val="204"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <t>cм</t>
-  </si>
-  <si>
-    <t>Дано</t>
-  </si>
-  <si>
-    <t>см</t>
-  </si>
-  <si>
-    <r>
-      <t>см</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Inter"/>
-        <charset val="204"/>
-      </rPr>
-      <t>4</t>
-    </r>
-  </si>
-  <si>
-    <t>кг/см</t>
-  </si>
-  <si>
-    <t>Расчёт</t>
-  </si>
-  <si>
-    <t>Норма</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>γ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>с</t>
-    </r>
-  </si>
-  <si>
-    <t>Ry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-  </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -498,58 +373,11 @@
       <charset val="204"/>
     </font>
     <font>
-      <b/>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
     </font>
     <font>
       <i/>
@@ -583,18 +411,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -769,65 +597,27 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -836,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -893,7 +683,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -903,112 +692,20 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1020,17 +717,56 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1394,20 +1130,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3645CFB6-B0BD-4446-9F44-E628F3BF8E11}" name="Таблица1" displayName="Таблица1" ref="A1:H7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3645CFB6-B0BD-4446-9F44-E628F3BF8E11}" name="Таблица1" displayName="Таблица1" ref="A1:H7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8183B60A-E10C-4A2E-92F1-AF84282C6280}" name="№ п/п" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{A9B5C510-C500-4B6B-A610-EE651E35788C}" name="Наименование" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{BD971CA7-2305-4C0C-839D-A359F4BD63F7}" name="ρ" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{41A4268E-525C-47E5-A064-5232788AFB22}" name="h" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{1A43476B-C444-4C63-905B-9532CA4DE150}" name="Qн, " dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{8183B60A-E10C-4A2E-92F1-AF84282C6280}" name="№ п/п" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{A9B5C510-C500-4B6B-A610-EE651E35788C}" name="Наименование" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{BD971CA7-2305-4C0C-839D-A359F4BD63F7}" name="ρ" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{41A4268E-525C-47E5-A064-5232788AFB22}" name="h" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{1A43476B-C444-4C63-905B-9532CA4DE150}" name="Qн, " dataDxfId="9">
       <calculatedColumnFormula>C2*D2/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{101A6059-660B-45D5-909E-4820653C046A}" name="γf" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{AF3EEBC6-68E0-4413-8258-2E8F49BDB9F4}" name="Qp" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{101A6059-660B-45D5-909E-4820653C046A}" name="γf" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{AF3EEBC6-68E0-4413-8258-2E8F49BDB9F4}" name="Qp" dataDxfId="7">
       <calculatedColumnFormula>E2*F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{F0C0D757-D5DD-47AF-812E-47A755CB3B6D}" name="№ ГОСТ" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{F0C0D757-D5DD-47AF-812E-47A755CB3B6D}" name="№ ГОСТ" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1679,7 +1415,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1696,28 +1432,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1895,23 +1631,23 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="23" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="22" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="22" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="13"/>
@@ -1936,30 +1672,30 @@
       <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="D10" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="25">
+      <c r="D10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="24">
         <f>SUM(Таблица1[Qн, ])</f>
         <v>270.95</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="25">
+      <c r="F10" s="23"/>
+      <c r="G10" s="24">
         <f>SUM(Таблица1[Qp])</f>
         <v>352.84500000000003</v>
       </c>
-      <c r="H10" s="61"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="24">
+      <c r="D11" s="23">
         <v>2</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="23">
         <f>D11*E10</f>
         <v>541.9</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24">
+      <c r="F11" s="23"/>
+      <c r="G11" s="23">
         <f>D11*G10</f>
         <v>705.69</v>
       </c>
@@ -1977,476 +1713,255 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DCDC94-8D65-44A4-8AE5-D87CCC3BD610}">
-  <dimension ref="A1:M14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9E8718-6AD5-4BAC-8B1F-72CAB04E655F}">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScale="178" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.77734375" style="21" customWidth="1"/>
-    <col min="10" max="12" width="8.77734375" style="21" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="21"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="36">
-        <f>(5/384)*(C3*D3^4)/(E3*G3)</f>
-        <v>317.21413764144273</v>
-      </c>
-      <c r="C3" s="36">
-        <f>СборНагрузок!E11/100</f>
-        <v>5.4189999999999996</v>
-      </c>
-      <c r="D3" s="32">
-        <v>600</v>
-      </c>
-      <c r="E3" s="32">
-        <f>200000000000/9.81/(100^2)</f>
-        <v>2038735.9836901119</v>
-      </c>
-      <c r="F3" s="36"/>
-      <c r="G3" s="55">
-        <v>14.14</v>
-      </c>
-      <c r="H3" s="55">
-        <v>50</v>
-      </c>
-      <c r="I3" s="56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="56"/>
-    </row>
-    <row r="5" spans="1:13" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="str">
-        <f>A2</f>
-        <v>Единица</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45"/>
-    </row>
-    <row r="8" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="38" t="str">
-        <f>IF(B3&lt;1/200*D3, J1, J2)</f>
-        <v>✗</v>
-      </c>
-      <c r="C8" s="57">
-        <v>5.66</v>
-      </c>
-      <c r="D8" s="26">
-        <f>C3*D3^2/8</f>
-        <v>243854.99999999997</v>
-      </c>
-      <c r="E8" s="26">
-        <f>D8/C8</f>
-        <v>43083.922261484091</v>
-      </c>
-      <c r="F8" s="38" t="str">
-        <f>IF(E8&lt;=G8, J1,J2)</f>
-        <v>✗</v>
-      </c>
-      <c r="G8" s="46">
-        <v>235</v>
-      </c>
-      <c r="H8" s="47"/>
-      <c r="I8" s="48"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="38" t="str">
-        <f>IF(B4&lt;1/200*D3, J1, J2)</f>
-        <v>✓</v>
-      </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="26">
-        <f>C4*D3^2/8</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="26">
-        <f>D9/C8</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="38" t="str">
-        <f>IF(E9&lt;=G8,J1,J2)</f>
-        <v>✓</v>
-      </c>
-      <c r="G9" s="49"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="51"/>
-    </row>
-    <row r="10" spans="1:13" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="42" t="str">
-        <f>J1&amp;"/"&amp;J2</f>
-        <v>✓/✗</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="42" t="str">
-        <f>B10</f>
-        <v>✓/✗</v>
-      </c>
-      <c r="G10" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="54"/>
-    </row>
-    <row r="11" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-    </row>
-    <row r="12" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="60"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-    </row>
-    <row r="13" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-    </row>
-    <row r="14" spans="1:13" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-    </row>
-  </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A11:I14"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I9"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9E8718-6AD5-4BAC-8B1F-72CAB04E655F}">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="21"/>
+    <col min="1" max="1" width="5.77734375" style="21" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="21"/>
+    <col min="3" max="3" width="8.88671875" style="21"/>
+    <col min="4" max="4" width="12" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A1" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="32">
+        <v>600</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="65">
-        <v>600</v>
-      </c>
-      <c r="C2" s="64" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="65">
-        <v>14.1</v>
-      </c>
-      <c r="C3" s="64" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="65">
-        <v>5.66</v>
-      </c>
-      <c r="C4" s="64" t="s">
-        <v>56</v>
-      </c>
+      <c r="B3" s="37">
+        <v>1581.56</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="38">
+        <v>159.80000000000001</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="27"/>
     </row>
     <row r="5" spans="1:4" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="65">
-        <f>200000000000/9.81/(100^2)</f>
+      <c r="A5" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="32">
+        <f>2*10^5*10^6/9.81/(100^2)</f>
         <v>2038735.9836901119</v>
       </c>
-      <c r="C5" s="64" t="s">
-        <v>52</v>
-      </c>
+      <c r="C5" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="27"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="65">
+      <c r="A6" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="32">
         <f>СборНагрузок!E11/100</f>
         <v>5.4189999999999996</v>
       </c>
-      <c r="C6" s="64" t="s">
-        <v>63</v>
-      </c>
+      <c r="C6" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="21">
+      <c r="A7" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="32">
         <v>0.9</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="31" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="63" t="s">
-        <v>67</v>
-      </c>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="8" spans="1:4" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="27">
+        <f>240*10.1971621297792</f>
+        <v>2447.3189111470078</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="62" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="66" t="s">
-        <v>65</v>
+      <c r="A9" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="33" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="65">
+      <c r="A10" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="32">
         <f>(5/384)*(B6*B2^4)/(B5*B3)</f>
-        <v>318.11403590425533</v>
-      </c>
-      <c r="C10" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="68">
+        <v>2.836065597416475</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="36">
         <f>B2/200</f>
         <v>3</v>
       </c>
     </row>
+    <row r="11" spans="1:4" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="32">
+        <f>(5*25/48)*B6*(B2^3)/B5</f>
+        <v>1495.1359687499998</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="27"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="32">
+        <f>B6*B2^2/8</f>
+        <v>243854.99999999997</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="27"/>
+    </row>
+    <row r="14" spans="1:4" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="32">
+        <f>B13/B4</f>
+        <v>1526.0012515644553</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="35" t="str">
+        <f>LEFT("&lt; "&amp;B15, 10)</f>
+        <v>&lt; 2202,587</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="str">
+        <f>A8&amp;"*"&amp;A7</f>
+        <v>Ry*γс</v>
+      </c>
+      <c r="B15" s="27">
+        <f>B7*B8</f>
+        <v>2202.587020032307</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="1:4" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="21">
+        <f>B6*B2^2/(8*B15)</f>
+        <v>110.71299239583422</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
   </mergeCells>
   <conditionalFormatting sqref="B10">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>$D$10</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+      <formula>$D$10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>$B$15</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>$B$15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>$B$4</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
-      <formula>$D$10</formula>
+      <formula>$B$4</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>